<commit_message>
improved .gitattributes and .gitconfig
</commit_message>
<xml_diff>
--- a/doc/test2.xlsx
+++ b/doc/test2.xlsx
@@ -1,37 +1,381 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="8175"/>
+    <workbookView windowWidth="14310" windowHeight="7275"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725" iterate="1"/>
+  <calcPr calcId="144525" iterate="1" iterateCount="100" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="21">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -39,9 +383,251 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -50,11 +636,58 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="1" builtinId="10"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9"/>
+    <cellStyle name="Virgule" xfId="3" builtinId="3"/>
+    <cellStyle name="60 % - Accent6" xfId="4" builtinId="52"/>
+    <cellStyle name="Calcul" xfId="5" builtinId="22"/>
+    <cellStyle name="Titre" xfId="6" builtinId="15"/>
+    <cellStyle name="Monétaire [0]" xfId="7" builtinId="7"/>
+    <cellStyle name="Monétaire" xfId="8" builtinId="4"/>
+    <cellStyle name="Milliers [0]" xfId="9" builtinId="6"/>
+    <cellStyle name="Cellule liée" xfId="10" builtinId="24"/>
+    <cellStyle name="Pourcentage" xfId="11" builtinId="5"/>
+    <cellStyle name="Lien hypertexte" xfId="12" builtinId="8"/>
+    <cellStyle name="Avertissement" xfId="13" builtinId="11"/>
+    <cellStyle name="CTexte explicatif" xfId="14" builtinId="53"/>
+    <cellStyle name="Titre 1" xfId="15" builtinId="16"/>
+    <cellStyle name="Titre 2" xfId="16" builtinId="17"/>
+    <cellStyle name="Accent1" xfId="17" builtinId="29"/>
+    <cellStyle name="Titre 3" xfId="18" builtinId="18"/>
+    <cellStyle name="Accent2" xfId="19" builtinId="33"/>
+    <cellStyle name="Titre 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Neutre" xfId="21" builtinId="28"/>
+    <cellStyle name="Entrée" xfId="22" builtinId="20"/>
+    <cellStyle name="40 % - Accent2" xfId="23" builtinId="35"/>
+    <cellStyle name="Sortie" xfId="24" builtinId="21"/>
+    <cellStyle name="Vérification de cellule" xfId="25" builtinId="23"/>
+    <cellStyle name="Total" xfId="26" builtinId="25"/>
+    <cellStyle name="Accent4" xfId="27" builtinId="41"/>
+    <cellStyle name="Satisfaisant" xfId="28" builtinId="26"/>
+    <cellStyle name="Insatisfaisant" xfId="29" builtinId="27"/>
+    <cellStyle name="20 % - Accent1" xfId="30" builtinId="30"/>
+    <cellStyle name="40 % - Accent1" xfId="31" builtinId="31"/>
+    <cellStyle name="60 % - Accent1" xfId="32" builtinId="32"/>
+    <cellStyle name="20 % - Accent2" xfId="33" builtinId="34"/>
+    <cellStyle name="60 % - Accent2" xfId="34" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="35" builtinId="37"/>
+    <cellStyle name="20 % - Accent3" xfId="36" builtinId="38"/>
+    <cellStyle name="40 % - Accent3" xfId="37" builtinId="39"/>
+    <cellStyle name="60 % - Accent3" xfId="38" builtinId="40"/>
+    <cellStyle name="20 % - Accent4" xfId="39" builtinId="42"/>
+    <cellStyle name="40 % - Accent4" xfId="40" builtinId="43"/>
+    <cellStyle name="60 % - Accent4" xfId="41" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="42" builtinId="45"/>
+    <cellStyle name="20 % - Accent5" xfId="43" builtinId="46"/>
+    <cellStyle name="40 % - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60 % - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="20 % - Accent6" xfId="47" builtinId="50"/>
+    <cellStyle name="40 % - Accent6" xfId="48" builtinId="51"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -342,48 +975,62 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelRow="1"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1">
         <v>123</v>
       </c>
     </row>
+    <row r="2" spans="1:1">
+      <c r="A2">
+        <v>456</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.74791666666666667" right="0.74791666666666667" top="0.98402777777777783" bottom="0.98402777777777783" header="0.51180555555555562" footer="0.51180555555555562"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555556" footer="0.511805555555556"/>
   <pageSetup paperSize="256" fitToWidth="0" fitToHeight="0" orientation="portrait" useFirstPageNumber="1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScaleSheetLayoutView="100" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75"/>
   <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555562" footer="0.51180555555555562"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="portrait" useFirstPageNumber="1" errors="NA"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScaleSheetLayoutView="100" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75"/>
   <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555562" footer="0.51180555555555562"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="portrait" useFirstPageNumber="1" errors="NA"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>

</xml_diff>